<commit_message>
--PIFSC Resource Inventory: Documentation Updates--
README.md was updated to reference the RIA technical documentation
docs\PRI Business Rule List.xlsx was updated with DB business rules
docs\todo.txt was updated to update items and indicate some have moved into the GitLab issue tracking for project management purposes
</commit_message>
<xml_diff>
--- a/docs/PRI Business Rule List.xlsx
+++ b/docs/PRI Business Rule List.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>Rule ID</t>
   </si>
@@ -161,6 +161,83 @@
   </si>
   <si>
     <t>No authentication is required for accessing the RIA system, it is provided as a read-only method for accessing project/resource information</t>
+  </si>
+  <si>
+    <t>Resource Tag Naming Conventions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The Tag Naming convention used to identify the given project resource's version.  The suffix is required to be a series of period-delimited numbers (e.g. for a naming convention of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>db_module_packager_v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the tag value of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>db_module_packager_v1.13.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is valid and will be parsed as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>version 1.13.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Resource Tag Naming Convention Parsing Algorithm</t>
+  </si>
+  <si>
+    <t>The period-delimited numeric string is extracted using a regular expression into separate numbers.  Depending on the occurrence of the numeric string the number is multiplied by 1000 to the occurrence number (starting at 0) to the total score.  This allows three digit numbers for each major, minor, patch, etc. number to be sorted correctly.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +603,7 @@
   <dimension ref="A1:R161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,7 +674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -608,9 +685,14 @@
         <f>CONCATENATE("PRI-DB-", REPT("0", 3-LEN(A2)), A2)</f>
         <v>PRI-DB-001</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <f>A2+1</f>
         <v>2</v>
@@ -622,7 +704,12 @@
         <f t="shared" ref="C3:C6" si="0">CONCATENATE("PRI-DB-", REPT("0", 3-LEN(A3)), A3)</f>
         <v>PRI-DB-002</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="D3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">

</xml_diff>